<commit_message>
Atualização automática de PORTAO.xlsx
</commit_message>
<xml_diff>
--- a/PORTAO.xlsx
+++ b/PORTAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{001791C3-1A54-4E87-88A9-C26A86CEEFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42C6F925-42BB-4B31-B103-CE2ECED7D181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1143,7 +1130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1204,30 +1191,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1245,7 +1208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1284,17 +1247,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1342,7 +1300,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{27C2BCA3-A91D-4223-B786-5567353E5B77}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{79B687DB-8211-400E-9FCB-37AD729123AC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1372,10 +1330,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E9BBB0F-3E5E-4CB7-9FE5-A45A432843EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{199301EF-3D49-47C9-8974-1D8F36E31E1D}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1413,7 +1371,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C235B13-DAC5-4459-9952-51B78F8C7A7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF67B51E-308C-4EDA-88AB-3F4525FC7578}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1476,7 +1434,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4EB31E3-0573-4441-B249-70B9F39A460C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E738F2-F951-41D2-9653-CC45D7523691}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1495,7 +1453,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDEB4F18-53F3-1CC5-FC2B-B994DEF1119E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1177750B-714B-80BF-682A-D4C236117095}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1544,7 +1502,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54AAE4AB-CC46-E702-4D6A-B2919DA77EFF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83FE9991-7E96-5C55-56E2-9FF1FAFF93B2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1563,7 +1521,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B55CC93-0CED-2555-166A-8F97AF435B30}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91421A40-571F-DF2A-575D-2A0FFAEDC77B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1594,7 +1552,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C44C43E1-4BDD-62D1-D344-7FC333BEA446}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D723E227-E97E-F127-03EF-A3BEA94959CE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1625,7 +1583,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10CE680F-8B83-BC35-D5CE-D4C323249EB4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3E3DC4F-81B7-3194-9EEB-8539E37C04E6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1668,7 +1626,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BD9EB36-34E1-4408-8CAC-08CD5D7AA7EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD27555D-2C06-4750-A987-A56190D66104}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1706,7 +1664,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01065075-B0E0-454F-B1E2-72AABAB2CCDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5384A0AA-5935-41CA-8B6B-417D0EE3DD9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1749,7 +1707,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{421A3B03-A5C1-49CA-8CBA-3EBED70C64E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC004B13-B7D7-4873-9D39-54E611A40D27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2062,7 +2020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C093B46-0F7E-4138-929A-D247CDA3DEED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59043B1C-B0DA-47BF-A6A8-D0332843CB7D}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2074,98 +2032,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="42"/>
-    <col min="6" max="6" width="2" style="42" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="42" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="42"/>
+    <col min="1" max="5" width="12.5703125" style="39"/>
+    <col min="6" max="6" width="2" style="39" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="39" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="41"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="41"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="41"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="41"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="41"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="41"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="41"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="41"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="41"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="41"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="41"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="41"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="41"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="41"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="41"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="41"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="41"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="41"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="41"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="41"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="41"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="41"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="41"/>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="41"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="41"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="41"/>
+      <c r="F26" s="38"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="41"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="41"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="41"/>
+      <c r="F29" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5431,19 +5389,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5477,46 +5435,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>284</v>
       </c>
     </row>
@@ -5524,7 +5482,7 @@
       <c r="A2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>453799</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5536,10 +5494,10 @@
       <c r="E2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>275.48</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>529.24</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5568,7 +5526,7 @@
       <c r="A3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>453800</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5580,10 +5538,10 @@
       <c r="E3" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>275.48</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>529.24</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5612,7 +5570,7 @@
       <c r="A4" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>453539</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5624,10 +5582,10 @@
       <c r="E4" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>275.48</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>529.24</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5666,14 +5624,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5704,46 +5662,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>302</v>
       </c>
     </row>
@@ -5768,54 +5726,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="25" t="s">
         <v>315</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5826,43 +5785,43 @@
       <c r="B2" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="28">
         <v>45170</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="29">
         <v>2247</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="30">
         <v>11580</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="30">
         <v>1719</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="31" t="s">
         <v>321</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="32" t="s">
         <v>322</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="32" t="s">
         <v>322</v>
       </c>
     </row>
@@ -5893,25 +5852,24 @@
       <c r="B1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="33" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="37">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="34">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="37">
         <v>131</v>
       </c>
-      <c r="F1" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="40">
-        <v>131</v>
-      </c>
-      <c r="C2" s="38">
+      <c r="C2" s="35">
         <v>8.6628752810474809E-3</v>
       </c>
     </row>

</xml_diff>